<commit_message>
added a new entry to the tabe
</commit_message>
<xml_diff>
--- a/Copy of L1-ex2 Template.xlsx
+++ b/Copy of L1-ex2 Template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="47">
   <si>
     <t>Entity</t>
   </si>
@@ -133,7 +133,28 @@
     <t>playlist</t>
   </si>
   <si>
+    <t>Playlist Track</t>
+  </si>
+  <si>
     <t>Musikland</t>
+  </si>
+  <si>
+    <t>playlisttrack</t>
+  </si>
+  <si>
+    <t>Track ID</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Invoice ID</t>
+  </si>
+  <si>
+    <t>invoice</t>
+  </si>
+  <si>
+    <t>invoiceid</t>
   </si>
 </sst>
 </file>
@@ -548,18 +569,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="22.719285714285714" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="20.433571428571426" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="22.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="15.290714285714287" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.25">
@@ -905,30 +926,56 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -939,13 +986,21 @@
       <c r="L11" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -958,7 +1013,7 @@
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -974,7 +1029,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -990,7 +1045,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1006,7 +1061,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1022,7 +1077,7 @@
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1038,7 +1093,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1054,7 +1109,7 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1070,7 +1125,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1086,7 +1141,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1102,7 +1157,7 @@
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1118,7 +1173,7 @@
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1134,7 +1189,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1150,7 +1205,7 @@
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1166,7 +1221,7 @@
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1182,7 +1237,7 @@
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1198,7 +1253,7 @@
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1214,7 +1269,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1230,7 +1285,7 @@
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1246,7 +1301,7 @@
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1262,7 +1317,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1278,7 +1333,7 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1294,7 +1349,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -1310,7 +1365,7 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1326,7 +1381,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -1342,7 +1397,7 @@
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1358,7 +1413,7 @@
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -1374,7 +1429,7 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1390,7 +1445,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1406,7 +1461,7 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -1422,7 +1477,7 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -1438,7 +1493,7 @@
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -1454,7 +1509,7 @@
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -1470,7 +1525,7 @@
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -1486,7 +1541,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -1502,7 +1557,7 @@
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -1518,7 +1573,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -1534,7 +1589,7 @@
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -1550,7 +1605,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -1566,7 +1621,7 @@
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1582,7 +1637,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -1598,7 +1653,7 @@
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1614,7 +1669,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -1630,7 +1685,7 @@
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1646,7 +1701,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -1662,7 +1717,7 @@
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -1678,7 +1733,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -1694,7 +1749,7 @@
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -1710,7 +1765,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -1726,7 +1781,7 @@
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -1742,7 +1797,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -1758,7 +1813,7 @@
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -1774,7 +1829,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -1790,7 +1845,7 @@
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>

</xml_diff>